<commit_message>
Formatted Sheets and included asset market values
</commit_message>
<xml_diff>
--- a/data/time_series/discount_rate_data_towers.xlsx
+++ b/data/time_series/discount_rate_data_towers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\UPS_MV\data\time_series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maddi\Documents\UPS_MV\data\time_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3498FCA7-A478-41FD-A83E-31779C80CABB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CD01B9-2B78-40A3-9414-FAAD08237D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31950" yWindow="1860" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{817400F5-5A4D-4E63-93ED-D635BC8755C3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{817400F5-5A4D-4E63-93ED-D635BC8755C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Retirement" sheetId="1" r:id="rId1"/>
@@ -397,18 +397,18 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>42369</v>
       </c>
@@ -416,7 +416,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42400</v>
       </c>
@@ -424,7 +424,7 @@
         <v>4.7366994569141264E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>42429</v>
       </c>
@@ -432,7 +432,7 @@
         <v>4.600286242179874E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>42460</v>
       </c>
@@ -440,7 +440,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>42490</v>
       </c>
@@ -448,7 +448,7 @@
         <v>4.3122489979540712E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>42521</v>
       </c>
@@ -456,7 +456,7 @@
         <v>4.346103787785352E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>42551</v>
       </c>
@@ -464,7 +464,7 @@
         <v>4.0599999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>42582</v>
       </c>
@@ -472,7 +472,7 @@
         <v>3.9221543431390553E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>42613</v>
       </c>
@@ -480,7 +480,7 @@
         <v>3.9382476817971759E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>42643</v>
       </c>
@@ -488,7 +488,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>42674</v>
       </c>
@@ -496,7 +496,7 @@
         <v>4.0980291838718153E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>42704</v>
       </c>
@@ -504,7 +504,7 @@
         <v>4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>42735</v>
       </c>
@@ -512,7 +512,7 @@
         <v>4.3700000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>42766</v>
       </c>
@@ -520,7 +520,7 @@
         <v>4.389708729633298E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>42794</v>
       </c>
@@ -528,7 +528,7 @@
         <v>4.2665992639938727E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>42825</v>
       </c>
@@ -536,7 +536,7 @@
         <v>4.36E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>42855</v>
       </c>
@@ -544,7 +544,7 @@
         <v>4.2673153340285923E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>42886</v>
       </c>
@@ -552,7 +552,7 @@
         <v>4.1526434404491587E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>42916</v>
       </c>
@@ -560,7 +560,7 @@
         <v>4.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>42947</v>
       </c>
@@ -568,7 +568,7 @@
         <v>4.0251759091500215E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>42978</v>
       </c>
@@ -576,7 +576,7 @@
         <v>3.9320507562816923E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>43008</v>
       </c>
@@ -584,7 +584,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>43039</v>
       </c>
@@ -592,7 +592,7 @@
         <v>3.9635394077231101E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>43069</v>
       </c>
@@ -600,7 +600,7 @@
         <v>3.9767015082352565E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>43100</v>
       </c>
@@ -608,7 +608,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>43131</v>
       </c>
@@ -616,7 +616,7 @@
         <v>4.0178116901478156E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>43159</v>
       </c>
@@ -624,7 +624,7 @@
         <v>4.245781568894004E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>43190</v>
       </c>
@@ -632,7 +632,7 @@
         <v>4.1200000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>43220</v>
       </c>
@@ -640,7 +640,7 @@
         <v>4.2451904293764137E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>43251</v>
       </c>
@@ -648,7 +648,7 @@
         <v>4.1866596850818026E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>43281</v>
       </c>
@@ -656,7 +656,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>43312</v>
       </c>
@@ -664,7 +664,7 @@
         <v>4.3647706912586709E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>43343</v>
       </c>
@@ -672,7 +672,7 @@
         <v>4.323693225367773E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>43373</v>
       </c>
@@ -680,7 +680,7 @@
         <v>4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>43404</v>
       </c>
@@ -688,7 +688,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>43434</v>
       </c>
@@ -696,7 +696,7 @@
         <v>4.6656289955308711E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>43465</v>
       </c>
@@ -704,7 +704,7 @@
         <v>4.48E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>43496</v>
       </c>
@@ -712,7 +712,7 @@
         <v>4.3055245047731595E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>43524</v>
       </c>
@@ -720,7 +720,7 @@
         <v>4.3531566410682836E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>43555</v>
       </c>
@@ -728,7 +728,7 @@
         <v>4.07E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>43585</v>
       </c>
@@ -736,7 +736,7 @@
         <v>4.1489864069518163E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>43616</v>
       </c>
@@ -744,7 +744,7 @@
         <v>3.9221451775881204E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43646</v>
       </c>
@@ -752,7 +752,7 @@
         <v>3.73E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43677</v>
       </c>
@@ -760,7 +760,7 @@
         <v>3.6611791938189267E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>43708</v>
       </c>
@@ -768,7 +768,7 @@
         <v>3.2323487297099343E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>43738</v>
       </c>
@@ -776,7 +776,7 @@
         <v>3.32E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>43769</v>
       </c>
@@ -784,7 +784,7 @@
         <v>3.3142277411032026E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>43799</v>
       </c>
@@ -792,7 +792,7 @@
         <v>3.3256110978756206E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>43830</v>
       </c>
@@ -800,7 +800,7 @@
         <v>3.5200000000000002E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>43861</v>
       </c>
@@ -808,7 +808,7 @@
         <v>3.2060660122441811E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>43890</v>
       </c>
@@ -816,7 +816,7 @@
         <v>3.0440818338531187E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>43921</v>
       </c>
@@ -824,7 +824,7 @@
         <v>3.61E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>43951</v>
       </c>
@@ -832,7 +832,7 @@
         <v>3.2263135185889566E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>43982</v>
       </c>
@@ -840,7 +840,7 @@
         <v>3.1678761714792669E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>44012</v>
       </c>
@@ -848,7 +848,7 @@
         <v>3.09E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>44043</v>
       </c>
@@ -856,7 +856,7 @@
         <v>2.7116463022710098E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>44074</v>
       </c>
@@ -864,7 +864,7 @@
         <v>3.0313574599253941E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>44104</v>
       </c>
@@ -872,7 +872,7 @@
         <v>3.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>44135</v>
       </c>
@@ -880,7 +880,7 @@
         <v>3.2037310216192647E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>44165</v>
       </c>
@@ -888,7 +888,7 @@
         <v>2.9548787340192752E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>44196</v>
       </c>
@@ -896,7 +896,7 @@
         <v>2.7699999999999999E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>44227</v>
       </c>
@@ -904,7 +904,7 @@
         <v>2.9774773686856732E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>44255</v>
       </c>
@@ -912,7 +912,7 @@
         <v>3.2444063265233414E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>44286</v>
       </c>
@@ -920,7 +920,7 @@
         <v>3.4500000000000003E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>44316</v>
       </c>
@@ -928,7 +928,7 @@
         <v>3.2899999999999999E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>44347</v>
       </c>
@@ -936,7 +936,7 @@
         <v>3.2709440329058599E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>44377</v>
       </c>
@@ -944,7 +944,7 @@
         <v>3.0499999999999999E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>44408</v>
       </c>
@@ -952,7 +952,7 @@
         <v>2.9139093747394231E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>44439</v>
       </c>
@@ -960,7 +960,7 @@
         <v>2.9659955142324987E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>44469</v>
       </c>
@@ -977,22 +977,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2C529B-40E9-4EAD-A980-83EC213AE0DF}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>42369</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42400</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>4.9093236496019203E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>42429</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>4.7665469359014306E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>42460</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>4.5499999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>42490</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>4.4572898985161008E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>42521</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>4.4877835292304775E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>42551</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>4.1700000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>42582</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>4.0265216873626934E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>42613</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>4.0260754166585921E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>42643</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>4.02E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>42674</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>4.2232318803501132E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>42704</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>4.5400000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>42735</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>42766</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>4.510071265525914E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>42794</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>4.3872135456713604E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>42825</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>42855</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>4.3857176352947849E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>42886</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>4.2664228419106255E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>42916</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>4.1399999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>42947</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>4.1212328493481484E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>42978</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>4.0308617030021685E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>43008</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>4.07E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>43039</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>4.0266023018670688E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>43069</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>4.0232663077605757E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>43100</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>3.8800000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>43131</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>4.0617936438227482E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>43159</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>4.2882072096180342E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>43190</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>43220</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>4.2812834735013176E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>43251</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>4.2247673778828834E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>43281</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>43312</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>4.3795461780044072E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>43343</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>4.3460211640645396E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>43373</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>4.4400000000000002E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>43404</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>43434</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>4.707815718379451E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>43465</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>4.5199999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>43496</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>4.365604318718385E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>43524</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>4.4139546137821249E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>43555</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>4.1300000000000003E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>43585</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>4.2115476139573095E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>43616</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>3.9870583792531E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43646</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43677</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>3.748182990029094E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>43708</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>3.3088949120622699E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>43738</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>3.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>43769</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>3.421720940868235E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>43799</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>3.4196812797862353E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>43830</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>3.7400000000000003E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>43861</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>3.4283330894466051E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>43890</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>3.2726530029998036E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>43921</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>3.8699999999999998E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>43951</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>3.5379670996363008E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>43982</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>3.5160823089304225E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>44012</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>44043</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>3.0089021513417358E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>44074</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>3.3546502582302101E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>44104</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>44135</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>3.5304536617438695E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>44165</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>3.2552993366350508E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>44196</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>3.1300000000000001E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>44227</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>3.3450267874524875E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>44255</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>3.6045438051028222E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>44286</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>3.7400000000000003E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>44316</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>3.5499999999999997E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>44347</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>3.5368552435727174E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>44377</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>3.2800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>44408</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>3.1487226086696816E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>44439</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>3.1968833410359401E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>44469</v>
       </c>
@@ -1561,21 +1561,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCEB45A-A12F-461B-B914-1C4E6556026A}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>42369</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42400</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>4.8851153635294041E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>42429</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>4.7455245037516795E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>42460</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>42490</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>4.3992140434594783E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>42521</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>4.4315357364001592E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>42551</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>4.1300000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>42582</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>3.9897858962699546E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>42613</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>3.9931161505142601E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>42643</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>3.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>42674</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>4.1705457382030936E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>42704</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>4.48E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>42735</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>4.4400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>42766</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>4.4597549945384569E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>42794</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>4.3378518635349042E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>42825</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>42855</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>4.3339196097317664E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>42886</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>4.2169177156466509E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>42916</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>42947</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>4.0789968780039709E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>42978</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>3.9889255441623875E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>43008</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>43039</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>3.9891948511617439E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>43069</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>3.9905869156692149E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>43100</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>3.8699999999999998E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>43131</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>4.0562973162394551E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>43159</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>4.2822433182052359E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>43190</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>43220</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>4.282165329182884E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>43251</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>4.2246050008553429E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>43281</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>43312</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>4.3813512393949143E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>43343</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>4.3454850371869358E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>43373</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>43404</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>43434</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>4.7373186573177788E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>43465</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>4.5199999999999997E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>43496</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>4.3604784783610351E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>43524</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>4.4082899887221867E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>43555</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>4.1200000000000001E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>43585</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>4.2004620594577637E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>43616</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>3.9760904206093781E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43646</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43677</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>3.7498752247637247E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>43708</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>3.3141569440769986E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>43738</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>3.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>43769</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>3.4192513828647506E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>43799</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>3.4207848896413914E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>43830</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>3.6499999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>43861</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>3.3385011571345984E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>43890</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>3.1815536906984486E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>43921</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>3.8399999999999997E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>43951</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>3.4968720647309534E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>43982</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>3.4643984803571316E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>44012</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>3.2800000000000003E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>44043</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>2.8949733525614862E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>44074</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>3.2316541812770161E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>44104</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>3.32E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>44135</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>3.4483239645572747E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>44165</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>3.1808909408023223E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>44196</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>2.98E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>44227</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>3.1915186686081003E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>44255</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>3.4504307130046909E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>44286</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>44316</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>3.5666389226273194E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>44347</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>3.5516854508816725E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>44377</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>3.2399999999999998E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>44408</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>3.1081783523249425E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>44439</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>3.1572979001821669E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>44469</v>
       </c>

</xml_diff>